<commit_message>
evaluate switch time in 100s add iperf.log
</commit_message>
<xml_diff>
--- a/Testbed/cmd/switch-throughput/result.xlsx
+++ b/Testbed/cmd/switch-throughput/result.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="100s" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -117,7 +118,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -450,11 +450,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="242307024"/>
-        <c:axId val="242305456"/>
+        <c:axId val="201176288"/>
+        <c:axId val="201174328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="242307024"/>
+        <c:axId val="201176288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -487,7 +487,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -554,7 +553,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242305456"/>
+        <c:crossAx val="201174328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -562,7 +561,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="242305456"/>
+        <c:axId val="201174328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -609,7 +608,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -670,7 +668,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242307024"/>
+        <c:crossAx val="201176288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -759,7 +757,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1092,11 +1089,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="399830872"/>
-        <c:axId val="399828128"/>
+        <c:axId val="201173152"/>
+        <c:axId val="201178640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="399830872"/>
+        <c:axId val="201173152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1129,7 +1126,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1196,7 +1192,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399828128"/>
+        <c:crossAx val="201178640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1204,7 +1200,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="399828128"/>
+        <c:axId val="201178640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1251,7 +1247,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1312,7 +1307,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399830872"/>
+        <c:crossAx val="201173152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1738,11 +1733,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="399819536"/>
-        <c:axId val="399820712"/>
+        <c:axId val="201172368"/>
+        <c:axId val="201173936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="399819536"/>
+        <c:axId val="201172368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1842,7 +1837,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399820712"/>
+        <c:crossAx val="201173936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1850,7 +1845,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="399820712"/>
+        <c:axId val="201173936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1958,7 +1953,1611 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399819536"/>
+        <c:crossAx val="201172368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Switch Bandwidth Effect</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'100s'!$A$1:$A$200</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="200"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>26.5</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>28.5</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>29.5</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>30.5</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>31.5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>33.5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>34.5</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>35.5</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>36.5</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>38.5</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>39.5</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>40.5</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>41.5</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>42.5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>43.5</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>44.5</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>45.5</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>46.5</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>47.5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>48.5</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>49.5</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>50.5</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>51.5</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>52.5</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>53.5</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>54.5</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>55.5</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>56.5</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>57.5</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>58.5</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>59.5</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>60.5</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>61.5</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>63.5</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>64.5</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>65.5</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>66.5</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>67.5</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>68.5</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>69.5</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>70.5</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>71.5</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>73.5</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>74.5</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>75.5</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>76.5</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>77.5</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>78.5</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>79.5</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>80.5</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>81.5</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>82.5</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>83.5</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>84.5</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>85.5</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>86.5</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>87.5</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>89.5</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>90.5</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>91.5</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>92.5</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>93.5</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>94.5</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>95.5</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>96.5</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>98.5</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>99.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'100s'!$B$1:$B$200</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="200"/>
+                <c:pt idx="0">
+                  <c:v>6978</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9418</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9421</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9421</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9420</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9418</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9420</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9417</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9413</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9419</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9417</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9413</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9412</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9421</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9417</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9410</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9419</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9413</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9416</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9413</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9416</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4874</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3232</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>9416</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>9416</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>9416</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>9418</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>9416</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>9411</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>9418</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>9413</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>9416</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>9412</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>9417</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>5597</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1652</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>9412</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>9417</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>9412</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>9413</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>9417</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>9411</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>9419</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>9411</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>9417</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>9413</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>9412</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>9418</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>5643</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>2474</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>9416</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>9413</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>9417</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>9416</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>9410</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>9419</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>9410</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>9419</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>5616</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>5409</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>9416</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>9412</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>9417</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>9413</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>9416</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>9412</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>9417</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>9412</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>9417</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>9415</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>9414</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>9411</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>9419</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>9414</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="402253088"/>
+        <c:axId val="402257792"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="402253088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Time(s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="402257792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="40"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="402257792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Bandwidth(Mbps)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="402253088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2127,6 +3726,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -3134,6 +4773,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3720,6 +5862,41 @@
       <xdr:colOff>200025</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>438151</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4706,7 +6883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
@@ -5037,4 +7214,1622 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B200"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>6978</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>0.5</v>
+      </c>
+      <c r="B2">
+        <v>9418</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>9421</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>1.5</v>
+      </c>
+      <c r="B4">
+        <v>9421</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>9420</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>2.5</v>
+      </c>
+      <c r="B6">
+        <v>9418</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>9420</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>3.5</v>
+      </c>
+      <c r="B8">
+        <v>9417</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>9413</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>4.5</v>
+      </c>
+      <c r="B10">
+        <v>9419</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>9417</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>5.5</v>
+      </c>
+      <c r="B12">
+        <v>9413</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>9412</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>6.5</v>
+      </c>
+      <c r="B14">
+        <v>9421</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>7.5</v>
+      </c>
+      <c r="B16">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>9417</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>8.5</v>
+      </c>
+      <c r="B18">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>9.5</v>
+      </c>
+      <c r="B20">
+        <v>9410</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <v>9419</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>10.5</v>
+      </c>
+      <c r="B22">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>11.5</v>
+      </c>
+      <c r="B24">
+        <v>9413</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>12</v>
+      </c>
+      <c r="B25">
+        <v>9416</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>12.5</v>
+      </c>
+      <c r="B26">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>13</v>
+      </c>
+      <c r="B27">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>13.5</v>
+      </c>
+      <c r="B28">
+        <v>9413</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A30">
+        <v>14.5</v>
+      </c>
+      <c r="B30">
+        <v>9416</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A31">
+        <v>15</v>
+      </c>
+      <c r="B31">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A32">
+        <v>15.5</v>
+      </c>
+      <c r="B32">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33">
+        <v>16</v>
+      </c>
+      <c r="B33">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A34">
+        <v>16.5</v>
+      </c>
+      <c r="B34">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A35">
+        <v>17</v>
+      </c>
+      <c r="B35">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A36">
+        <v>17.5</v>
+      </c>
+      <c r="B36">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A37">
+        <v>18</v>
+      </c>
+      <c r="B37">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A38">
+        <v>18.5</v>
+      </c>
+      <c r="B38">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A39">
+        <v>19</v>
+      </c>
+      <c r="B39">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A40">
+        <v>19.5</v>
+      </c>
+      <c r="B40">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>20</v>
+      </c>
+      <c r="B41">
+        <v>4874</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A42">
+        <v>20.5</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A43">
+        <v>21</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A44">
+        <v>21.5</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A45">
+        <v>22</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A46">
+        <v>22.5</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A47">
+        <v>23</v>
+      </c>
+      <c r="B47">
+        <v>3232</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A48">
+        <v>23.5</v>
+      </c>
+      <c r="B48">
+        <v>9416</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A49">
+        <v>24</v>
+      </c>
+      <c r="B49">
+        <v>9416</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A50">
+        <v>24.5</v>
+      </c>
+      <c r="B50">
+        <v>9416</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A51">
+        <v>25</v>
+      </c>
+      <c r="B51">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A52">
+        <v>25.5</v>
+      </c>
+      <c r="B52">
+        <v>9418</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A53">
+        <v>26</v>
+      </c>
+      <c r="B53">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A54">
+        <v>26.5</v>
+      </c>
+      <c r="B54">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A55">
+        <v>27</v>
+      </c>
+      <c r="B55">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A56">
+        <v>27.5</v>
+      </c>
+      <c r="B56">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A57">
+        <v>28</v>
+      </c>
+      <c r="B57">
+        <v>9416</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A58">
+        <v>28.5</v>
+      </c>
+      <c r="B58">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A59">
+        <v>29</v>
+      </c>
+      <c r="B59">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A60">
+        <v>29.5</v>
+      </c>
+      <c r="B60">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A61">
+        <v>30</v>
+      </c>
+      <c r="B61">
+        <v>9411</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A62">
+        <v>30.5</v>
+      </c>
+      <c r="B62">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A63">
+        <v>31</v>
+      </c>
+      <c r="B63">
+        <v>9418</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A64">
+        <v>31.5</v>
+      </c>
+      <c r="B64">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A65">
+        <v>32</v>
+      </c>
+      <c r="B65">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A66">
+        <v>32.5</v>
+      </c>
+      <c r="B66">
+        <v>9413</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A67">
+        <v>33</v>
+      </c>
+      <c r="B67">
+        <v>9416</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A68">
+        <v>33.5</v>
+      </c>
+      <c r="B68">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A69">
+        <v>34</v>
+      </c>
+      <c r="B69">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A70">
+        <v>34.5</v>
+      </c>
+      <c r="B70">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A71">
+        <v>35</v>
+      </c>
+      <c r="B71">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A72">
+        <v>35.5</v>
+      </c>
+      <c r="B72">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A73">
+        <v>36</v>
+      </c>
+      <c r="B73">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A74">
+        <v>36.5</v>
+      </c>
+      <c r="B74">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A75">
+        <v>37</v>
+      </c>
+      <c r="B75">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A76">
+        <v>37.5</v>
+      </c>
+      <c r="B76">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A77">
+        <v>38</v>
+      </c>
+      <c r="B77">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A78">
+        <v>38.5</v>
+      </c>
+      <c r="B78">
+        <v>9412</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A79">
+        <v>39</v>
+      </c>
+      <c r="B79">
+        <v>9417</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A80">
+        <v>39.5</v>
+      </c>
+      <c r="B80">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A81">
+        <v>40</v>
+      </c>
+      <c r="B81">
+        <v>5597</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A82">
+        <v>40.5</v>
+      </c>
+      <c r="B82">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A83">
+        <v>41</v>
+      </c>
+      <c r="B83">
+        <v>9412</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A84">
+        <v>41.5</v>
+      </c>
+      <c r="B84">
+        <v>9417</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A85">
+        <v>42</v>
+      </c>
+      <c r="B85">
+        <v>9412</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A86">
+        <v>42.5</v>
+      </c>
+      <c r="B86">
+        <v>9413</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A87">
+        <v>43</v>
+      </c>
+      <c r="B87">
+        <v>9417</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A88">
+        <v>43.5</v>
+      </c>
+      <c r="B88">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A89">
+        <v>44</v>
+      </c>
+      <c r="B89">
+        <v>9411</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A90">
+        <v>44.5</v>
+      </c>
+      <c r="B90">
+        <v>9419</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A91">
+        <v>45</v>
+      </c>
+      <c r="B91">
+        <v>9411</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A92">
+        <v>45.5</v>
+      </c>
+      <c r="B92">
+        <v>9417</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A93">
+        <v>46</v>
+      </c>
+      <c r="B93">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A94">
+        <v>46.5</v>
+      </c>
+      <c r="B94">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A95">
+        <v>47</v>
+      </c>
+      <c r="B95">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A96">
+        <v>47.5</v>
+      </c>
+      <c r="B96">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A97">
+        <v>48</v>
+      </c>
+      <c r="B97">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A98">
+        <v>48.5</v>
+      </c>
+      <c r="B98">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A99">
+        <v>49</v>
+      </c>
+      <c r="B99">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A100">
+        <v>49.5</v>
+      </c>
+      <c r="B100">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A101">
+        <v>50</v>
+      </c>
+      <c r="B101">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A102">
+        <v>50.5</v>
+      </c>
+      <c r="B102">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A103">
+        <v>51</v>
+      </c>
+      <c r="B103">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A104">
+        <v>51.5</v>
+      </c>
+      <c r="B104">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A105">
+        <v>52</v>
+      </c>
+      <c r="B105">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A106">
+        <v>52.5</v>
+      </c>
+      <c r="B106">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A107">
+        <v>53</v>
+      </c>
+      <c r="B107">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A108">
+        <v>53.5</v>
+      </c>
+      <c r="B108">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A109">
+        <v>54</v>
+      </c>
+      <c r="B109">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A110">
+        <v>54.5</v>
+      </c>
+      <c r="B110">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A111">
+        <v>55</v>
+      </c>
+      <c r="B111">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A112">
+        <v>55.5</v>
+      </c>
+      <c r="B112">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A113">
+        <v>56</v>
+      </c>
+      <c r="B113">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A114">
+        <v>56.5</v>
+      </c>
+      <c r="B114">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A115">
+        <v>57</v>
+      </c>
+      <c r="B115">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A116">
+        <v>57.5</v>
+      </c>
+      <c r="B116">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A117">
+        <v>58</v>
+      </c>
+      <c r="B117">
+        <v>9413</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A118">
+        <v>58.5</v>
+      </c>
+      <c r="B118">
+        <v>9412</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A119">
+        <v>59</v>
+      </c>
+      <c r="B119">
+        <v>9418</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A120">
+        <v>59.5</v>
+      </c>
+      <c r="B120">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A121">
+        <v>60</v>
+      </c>
+      <c r="B121">
+        <v>5643</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A122">
+        <v>60.5</v>
+      </c>
+      <c r="B122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A123">
+        <v>61</v>
+      </c>
+      <c r="B123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A124">
+        <v>61.5</v>
+      </c>
+      <c r="B124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A125">
+        <v>62</v>
+      </c>
+      <c r="B125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A126">
+        <v>62.5</v>
+      </c>
+      <c r="B126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A127">
+        <v>63</v>
+      </c>
+      <c r="B127">
+        <v>2474</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A128">
+        <v>63.5</v>
+      </c>
+      <c r="B128">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A129">
+        <v>64</v>
+      </c>
+      <c r="B129">
+        <v>9416</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A130">
+        <v>64.5</v>
+      </c>
+      <c r="B130">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A131">
+        <v>65</v>
+      </c>
+      <c r="B131">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A132">
+        <v>65.5</v>
+      </c>
+      <c r="B132">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A133">
+        <v>66</v>
+      </c>
+      <c r="B133">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A134">
+        <v>66.5</v>
+      </c>
+      <c r="B134">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A135">
+        <v>67</v>
+      </c>
+      <c r="B135">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A136">
+        <v>67.5</v>
+      </c>
+      <c r="B136">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A137">
+        <v>68</v>
+      </c>
+      <c r="B137">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A138">
+        <v>68.5</v>
+      </c>
+      <c r="B138">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A139">
+        <v>69</v>
+      </c>
+      <c r="B139">
+        <v>9413</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A140">
+        <v>69.5</v>
+      </c>
+      <c r="B140">
+        <v>9417</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A141">
+        <v>70</v>
+      </c>
+      <c r="B141">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A142">
+        <v>70.5</v>
+      </c>
+      <c r="B142">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A143">
+        <v>71</v>
+      </c>
+      <c r="B143">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A144">
+        <v>71.5</v>
+      </c>
+      <c r="B144">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A145">
+        <v>72</v>
+      </c>
+      <c r="B145">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A146">
+        <v>72.5</v>
+      </c>
+      <c r="B146">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A147">
+        <v>73</v>
+      </c>
+      <c r="B147">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A148">
+        <v>73.5</v>
+      </c>
+      <c r="B148">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A149">
+        <v>74</v>
+      </c>
+      <c r="B149">
+        <v>9416</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A150">
+        <v>74.5</v>
+      </c>
+      <c r="B150">
+        <v>9410</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A151">
+        <v>75</v>
+      </c>
+      <c r="B151">
+        <v>9419</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A152">
+        <v>75.5</v>
+      </c>
+      <c r="B152">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A153">
+        <v>76</v>
+      </c>
+      <c r="B153">
+        <v>9410</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A154">
+        <v>76.5</v>
+      </c>
+      <c r="B154">
+        <v>9419</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A155">
+        <v>77</v>
+      </c>
+      <c r="B155">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A156">
+        <v>77.5</v>
+      </c>
+      <c r="B156">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A157">
+        <v>78</v>
+      </c>
+      <c r="B157">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A158">
+        <v>78.5</v>
+      </c>
+      <c r="B158">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A159">
+        <v>79</v>
+      </c>
+      <c r="B159">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A160">
+        <v>79.5</v>
+      </c>
+      <c r="B160">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A161">
+        <v>80</v>
+      </c>
+      <c r="B161">
+        <v>5616</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A162">
+        <v>80.5</v>
+      </c>
+      <c r="B162">
+        <v>5409</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A163">
+        <v>81</v>
+      </c>
+      <c r="B163">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A164">
+        <v>81.5</v>
+      </c>
+      <c r="B164">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A165">
+        <v>82</v>
+      </c>
+      <c r="B165">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A166">
+        <v>82.5</v>
+      </c>
+      <c r="B166">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A167">
+        <v>83</v>
+      </c>
+      <c r="B167">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A168">
+        <v>83.5</v>
+      </c>
+      <c r="B168">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A169">
+        <v>84</v>
+      </c>
+      <c r="B169">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A170">
+        <v>84.5</v>
+      </c>
+      <c r="B170">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A171">
+        <v>85</v>
+      </c>
+      <c r="B171">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A172">
+        <v>85.5</v>
+      </c>
+      <c r="B172">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A173">
+        <v>86</v>
+      </c>
+      <c r="B173">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A174">
+        <v>86.5</v>
+      </c>
+      <c r="B174">
+        <v>9416</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A175">
+        <v>87</v>
+      </c>
+      <c r="B175">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A176">
+        <v>87.5</v>
+      </c>
+      <c r="B176">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A177">
+        <v>88</v>
+      </c>
+      <c r="B177">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A178">
+        <v>88.5</v>
+      </c>
+      <c r="B178">
+        <v>9412</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A179">
+        <v>89</v>
+      </c>
+      <c r="B179">
+        <v>9417</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A180">
+        <v>89.5</v>
+      </c>
+      <c r="B180">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A181">
+        <v>90</v>
+      </c>
+      <c r="B181">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A182">
+        <v>90.5</v>
+      </c>
+      <c r="B182">
+        <v>9413</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A183">
+        <v>91</v>
+      </c>
+      <c r="B183">
+        <v>9416</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A184">
+        <v>91.5</v>
+      </c>
+      <c r="B184">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A185">
+        <v>92</v>
+      </c>
+      <c r="B185">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A186">
+        <v>92.5</v>
+      </c>
+      <c r="B186">
+        <v>9412</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A187">
+        <v>93</v>
+      </c>
+      <c r="B187">
+        <v>9417</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A188">
+        <v>93.5</v>
+      </c>
+      <c r="B188">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A189">
+        <v>94</v>
+      </c>
+      <c r="B189">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A190">
+        <v>94.5</v>
+      </c>
+      <c r="B190">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A191">
+        <v>95</v>
+      </c>
+      <c r="B191">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A192">
+        <v>95.5</v>
+      </c>
+      <c r="B192">
+        <v>9412</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A193">
+        <v>96</v>
+      </c>
+      <c r="B193">
+        <v>9417</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A194">
+        <v>96.5</v>
+      </c>
+      <c r="B194">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A195">
+        <v>97</v>
+      </c>
+      <c r="B195">
+        <v>9415</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A196">
+        <v>97.5</v>
+      </c>
+      <c r="B196">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A197">
+        <v>98</v>
+      </c>
+      <c r="B197">
+        <v>9414</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A198">
+        <v>98.5</v>
+      </c>
+      <c r="B198">
+        <v>9411</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A199">
+        <v>99</v>
+      </c>
+      <c r="B199">
+        <v>9419</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A200">
+        <v>99.5</v>
+      </c>
+      <c r="B200">
+        <v>9414</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>